<commit_message>
Add results of KDI shocks
</commit_message>
<xml_diff>
--- a/energy_data/xlsx_data/KDI_supply_shocks.xlsx
+++ b/energy_data/xlsx_data/KDI_supply_shocks.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="gasoline" sheetId="3" r:id="rId1"/>
+    <sheet name="gasoline" sheetId="5" r:id="rId1"/>
     <sheet name="electricity" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211" concurrentCalc="0"/>
@@ -250,12 +250,12 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -263,12 +263,12 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="14"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -288,10 +288,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:F20" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table3" displayName="Table3" ref="A1:F20" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:F20"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Feedstock" dataDxfId="3"/>
+    <tableColumn id="1" name="Feedstock" dataDxfId="0"/>
     <tableColumn id="2" name="Technology"/>
     <tableColumn id="3" name="Quantity (MatLab)"/>
     <tableColumn id="4" name="Unit"/>
@@ -303,10 +303,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="A1:F38" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="A1:F38" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:F38"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Feedstock" dataDxfId="0"/>
+    <tableColumn id="1" name="Feedstock" dataDxfId="2"/>
     <tableColumn id="2" name="Technology"/>
     <tableColumn id="3" name="Quantity (MatLab)"/>
     <tableColumn id="4" name="Unit"/>
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,7 +993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>

</xml_diff>